<commit_message>
In progress CLS+Thủ Thuật
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Khám_bệnh.xlsx
+++ b/DataTest/Data_API_Khám_bệnh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thanh Truc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIS api automation\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8497DFC-02D3-4B78-A0A9-5A6466F8F0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE34CDC4-323D-4591-9FE6-94219DB36FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A137F98-0BBA-4431-A6F3-B324DFC003E1}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="18984" windowHeight="8880" xr2:uid="{7A137F98-0BBA-4431-A6F3-B324DFC003E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="94">
   <si>
     <t>MedServiceId</t>
   </si>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D377DE53-CCB9-4C13-9CB8-315A2AA61C2E}">
   <dimension ref="A1:CD121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BC3" sqref="BC3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BW8" sqref="BW8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1174,205 +1174,11 @@
       </c>
     </row>
     <row r="3" spans="1:82" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3">
-        <v>3839</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-      <c r="N3">
-        <v>17437</v>
-      </c>
-      <c r="O3" t="s">
-        <v>91</v>
-      </c>
       <c r="P3" s="2"/>
-      <c r="Q3">
-        <v>4803</v>
-      </c>
-      <c r="R3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3">
-        <v>13</v>
-      </c>
-      <c r="T3">
-        <v>13</v>
-      </c>
-      <c r="U3">
-        <v>30</v>
-      </c>
-      <c r="V3">
-        <v>130</v>
-      </c>
-      <c r="W3">
-        <v>2</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB3">
-        <v>1024</v>
-      </c>
-      <c r="AC3">
-        <v>7.1897000000000002</v>
-      </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
-      <c r="AE3">
-        <v>37500</v>
-      </c>
-      <c r="AF3">
-        <v>37500</v>
-      </c>
-      <c r="AG3">
-        <v>1083660</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
-      <c r="AP3">
-        <v>1</v>
-      </c>
-      <c r="AQ3">
-        <v>1</v>
-      </c>
-      <c r="AR3">
-        <v>392</v>
-      </c>
-      <c r="AS3">
-        <v>1084741</v>
-      </c>
-      <c r="AT3">
-        <v>1</v>
-      </c>
-      <c r="AU3">
-        <v>68300</v>
-      </c>
-      <c r="AV3">
-        <v>68300</v>
-      </c>
-      <c r="AW3">
-        <v>100</v>
-      </c>
-      <c r="AX3">
-        <v>552</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="AZ3">
-        <v>2</v>
-      </c>
-      <c r="BA3">
-        <v>6</v>
-      </c>
-      <c r="BB3">
-        <v>25</v>
-      </c>
-      <c r="BC3" t="b">
-        <v>0</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>83</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>84</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>85</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>86</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>89</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BO3">
-        <v>0</v>
-      </c>
-      <c r="BP3">
-        <v>1</v>
-      </c>
-      <c r="BU3">
-        <v>0</v>
-      </c>
-      <c r="BV3">
-        <v>0</v>
-      </c>
-      <c r="BW3">
-        <v>0</v>
-      </c>
-      <c r="BX3">
-        <v>13660</v>
-      </c>
-      <c r="BY3">
-        <v>0</v>
-      </c>
-      <c r="BZ3">
-        <v>54640</v>
-      </c>
-      <c r="CA3">
-        <v>0</v>
-      </c>
-      <c r="CB3">
-        <v>0</v>
-      </c>
+      <c r="AB3"/>
     </row>
     <row r="4" spans="1:82" x14ac:dyDescent="0.3">
       <c r="AB4"/>

</xml_diff>

<commit_message>
Fixbug tự động generate khám bệnh + CDDV
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Khám_bệnh.xlsx
+++ b/DataTest/Data_API_Khám_bệnh.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CD6"/>
+  <dimension ref="A1:CD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1357,774 +1357,6 @@
       <c r="CC3" t="inlineStr"/>
       <c r="CD3" t="inlineStr"/>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>3839</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2</v>
-      </c>
-      <c r="N4" t="n">
-        <v>17437</v>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Quách Bảo Hưng</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="n">
-        <v>4803</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>knt1</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>13</v>
-      </c>
-      <c r="T4" t="n">
-        <v>13</v>
-      </c>
-      <c r="U4" t="n">
-        <v>30</v>
-      </c>
-      <c r="V4" t="n">
-        <v>130</v>
-      </c>
-      <c r="W4" t="n">
-        <v>2</v>
-      </c>
-      <c r="X4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>Lần</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>Khám Nội Tiết 1</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>Khám Nội tiết</t>
-        </is>
-      </c>
-      <c r="AB4" t="n">
-        <v>1024</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>7.1897</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>1083660</v>
-      </c>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>17437|983307|149|10/05/2024 01:02|A00.9|Bệnh tả, không đặc hiệu|3839|3|10/05/2024 01:02|3839||||PendingProcessing|4803|80||Bệnh tả, không đặc hiệu|2|1083660|13||</t>
-        </is>
-      </c>
-      <c r="AL4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>392</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>1084741</v>
-      </c>
-      <c r="AT4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>68300</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>68300</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>100</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>552</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>6</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>25</v>
-      </c>
-      <c r="BC4" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD4" t="inlineStr"/>
-      <c r="BE4" t="inlineStr">
-        <is>
-          <t>XQ1</t>
-        </is>
-      </c>
-      <c r="BF4" t="inlineStr">
-        <is>
-          <t>Phòng X quang</t>
-        </is>
-      </c>
-      <c r="BG4" t="inlineStr">
-        <is>
-          <t>Chẩn đoán hình ảnh</t>
-        </is>
-      </c>
-      <c r="BH4" t="inlineStr">
-        <is>
-          <t>X-Quang</t>
-        </is>
-      </c>
-      <c r="BI4" t="inlineStr">
-        <is>
-          <t>xqm242</t>
-        </is>
-      </c>
-      <c r="BJ4" t="inlineStr">
-        <is>
-          <t>Chụp Xquang cột sống cổ chếch hai bên</t>
-        </is>
-      </c>
-      <c r="BK4" t="inlineStr">
-        <is>
-          <t>BHYT</t>
-        </is>
-      </c>
-      <c r="BL4" t="inlineStr"/>
-      <c r="BM4" t="inlineStr">
-        <is>
-          <t>Chờ thanh toán</t>
-        </is>
-      </c>
-      <c r="BN4" t="inlineStr">
-        <is>
-          <t>Chờ thanh toán</t>
-        </is>
-      </c>
-      <c r="BO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ4" t="inlineStr"/>
-      <c r="BR4" t="inlineStr"/>
-      <c r="BS4" t="inlineStr"/>
-      <c r="BT4" t="inlineStr"/>
-      <c r="BU4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>13660</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>54640</v>
-      </c>
-      <c r="CA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB4" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC4" t="inlineStr"/>
-      <c r="CD4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>3839</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" t="n">
-        <v>2</v>
-      </c>
-      <c r="N5" t="n">
-        <v>17437</v>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Quách Bảo Hưng</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="n">
-        <v>4803</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>knt1</t>
-        </is>
-      </c>
-      <c r="S5" t="n">
-        <v>13</v>
-      </c>
-      <c r="T5" t="n">
-        <v>13</v>
-      </c>
-      <c r="U5" t="n">
-        <v>30</v>
-      </c>
-      <c r="V5" t="n">
-        <v>130</v>
-      </c>
-      <c r="W5" t="n">
-        <v>2</v>
-      </c>
-      <c r="X5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>Lần</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>Khám Nội Tiết 1</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>Khám Nội tiết</t>
-        </is>
-      </c>
-      <c r="AB5" t="n">
-        <v>1024</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>7.1897</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>1083660</v>
-      </c>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>17437|983307|149|10/05/2024 01:02|A00.9|Bệnh tả, không đặc hiệu|3839|3|10/05/2024 01:02|3839||||PendingProcessing|4803|80||Bệnh tả, không đặc hiệu|2|1083660|13||</t>
-        </is>
-      </c>
-      <c r="AL5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>392</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>1084741</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>68300</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>68300</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>100</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>552</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>2</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>6</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>25</v>
-      </c>
-      <c r="BC5" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD5" t="inlineStr"/>
-      <c r="BE5" t="inlineStr">
-        <is>
-          <t>XQ1</t>
-        </is>
-      </c>
-      <c r="BF5" t="inlineStr">
-        <is>
-          <t>Phòng X quang</t>
-        </is>
-      </c>
-      <c r="BG5" t="inlineStr">
-        <is>
-          <t>Chẩn đoán hình ảnh</t>
-        </is>
-      </c>
-      <c r="BH5" t="inlineStr">
-        <is>
-          <t>X-Quang</t>
-        </is>
-      </c>
-      <c r="BI5" t="inlineStr">
-        <is>
-          <t>xqm242</t>
-        </is>
-      </c>
-      <c r="BJ5" t="inlineStr">
-        <is>
-          <t>Chụp Xquang cột sống cổ chếch hai bên</t>
-        </is>
-      </c>
-      <c r="BK5" t="inlineStr">
-        <is>
-          <t>BHYT</t>
-        </is>
-      </c>
-      <c r="BL5" t="inlineStr"/>
-      <c r="BM5" t="inlineStr">
-        <is>
-          <t>Chờ thanh toán</t>
-        </is>
-      </c>
-      <c r="BN5" t="inlineStr">
-        <is>
-          <t>Chờ thanh toán</t>
-        </is>
-      </c>
-      <c r="BO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ5" t="inlineStr"/>
-      <c r="BR5" t="inlineStr"/>
-      <c r="BS5" t="inlineStr"/>
-      <c r="BT5" t="inlineStr"/>
-      <c r="BU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX5" t="n">
-        <v>13660</v>
-      </c>
-      <c r="BY5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ5" t="n">
-        <v>54640</v>
-      </c>
-      <c r="CA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC5" t="inlineStr"/>
-      <c r="CD5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>A00.9</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Bệnh tả, không đặc hiệu</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>3839</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>17437</v>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Quách Bảo Hưng</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="n">
-        <v>4803</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>knt1</t>
-        </is>
-      </c>
-      <c r="S6" t="n">
-        <v>13</v>
-      </c>
-      <c r="T6" t="n">
-        <v>13</v>
-      </c>
-      <c r="U6" t="n">
-        <v>30</v>
-      </c>
-      <c r="V6" t="n">
-        <v>130</v>
-      </c>
-      <c r="W6" t="n">
-        <v>2</v>
-      </c>
-      <c r="X6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>Lần</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>Khám Nội Tiết 1</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>Khám Nội tiết</t>
-        </is>
-      </c>
-      <c r="AB6" t="n">
-        <v>1024</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>7.1897</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>37500</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>1083660</v>
-      </c>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>17437|983307|149|10/05/2024 01:02|A00.9|Bệnh tả, không đặc hiệu|3839|3|10/05/2024 01:02|3839||||PendingProcessing|4803|80||Bệnh tả, không đặc hiệu|2|1083660|13||</t>
-        </is>
-      </c>
-      <c r="AL6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>Re</t>
-        </is>
-      </c>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>392</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>1084741</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU6" t="n">
-        <v>68300</v>
-      </c>
-      <c r="AV6" t="n">
-        <v>68300</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>100</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>552</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AZ6" t="n">
-        <v>2</v>
-      </c>
-      <c r="BA6" t="n">
-        <v>6</v>
-      </c>
-      <c r="BB6" t="n">
-        <v>25</v>
-      </c>
-      <c r="BC6" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD6" t="inlineStr"/>
-      <c r="BE6" t="inlineStr">
-        <is>
-          <t>XQ1</t>
-        </is>
-      </c>
-      <c r="BF6" t="inlineStr">
-        <is>
-          <t>Phòng X quang</t>
-        </is>
-      </c>
-      <c r="BG6" t="inlineStr">
-        <is>
-          <t>Chẩn đoán hình ảnh</t>
-        </is>
-      </c>
-      <c r="BH6" t="inlineStr">
-        <is>
-          <t>X-Quang</t>
-        </is>
-      </c>
-      <c r="BI6" t="inlineStr">
-        <is>
-          <t>xqm242</t>
-        </is>
-      </c>
-      <c r="BJ6" t="inlineStr">
-        <is>
-          <t>Chụp Xquang cột sống cổ chếch hai bên</t>
-        </is>
-      </c>
-      <c r="BK6" t="inlineStr">
-        <is>
-          <t>BHYT</t>
-        </is>
-      </c>
-      <c r="BL6" t="inlineStr"/>
-      <c r="BM6" t="inlineStr">
-        <is>
-          <t>Chờ thanh toán</t>
-        </is>
-      </c>
-      <c r="BN6" t="inlineStr">
-        <is>
-          <t>Chờ thanh toán</t>
-        </is>
-      </c>
-      <c r="BO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP6" t="n">
-        <v>1</v>
-      </c>
-      <c r="BQ6" t="inlineStr"/>
-      <c r="BR6" t="inlineStr"/>
-      <c r="BS6" t="inlineStr"/>
-      <c r="BT6" t="inlineStr"/>
-      <c r="BU6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BV6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX6" t="n">
-        <v>13660</v>
-      </c>
-      <c r="BY6" t="n">
-        <v>0</v>
-      </c>
-      <c r="BZ6" t="n">
-        <v>54640</v>
-      </c>
-      <c r="CA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="CC6" t="inlineStr"/>
-      <c r="CD6" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Done tự động generate Viện phí
</commit_message>
<xml_diff>
--- a/DataTest/Data_API_Khám_bệnh.xlsx
+++ b/DataTest/Data_API_Khám_bệnh.xlsx
@@ -953,7 +953,7 @@
         <v>37500</v>
       </c>
       <c r="AG2" t="n">
-        <v>1083660</v>
+        <v>1094172</v>
       </c>
       <c r="AH2" t="inlineStr"/>
       <c r="AI2" t="inlineStr"/>
@@ -982,19 +982,19 @@
         <v>1</v>
       </c>
       <c r="AR2" t="n">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="AS2" t="n">
-        <v>1084741</v>
+        <v>1095239</v>
       </c>
       <c r="AT2" t="n">
         <v>1</v>
       </c>
       <c r="AU2" t="n">
-        <v>68300</v>
+        <v>624000</v>
       </c>
       <c r="AV2" t="n">
-        <v>68300</v>
+        <v>624000</v>
       </c>
       <c r="AW2" t="n">
         <v>100</v>
@@ -1040,12 +1040,12 @@
       </c>
       <c r="BI2" t="inlineStr">
         <is>
-          <t>xqm242</t>
+          <t>xq03</t>
         </is>
       </c>
       <c r="BJ2" t="inlineStr">
         <is>
-          <t>Chụp Xquang cột sống cổ chếch hai bên</t>
+          <t>Chụp Xquang bể thận-niệu quản xuôi dòng [Số hóa]</t>
         </is>
       </c>
       <c r="BK2" t="inlineStr">
@@ -1084,13 +1084,13 @@
         <v>0</v>
       </c>
       <c r="BX2" t="n">
-        <v>13660</v>
+        <v>124800</v>
       </c>
       <c r="BY2" t="n">
         <v>0</v>
       </c>
       <c r="BZ2" t="n">
-        <v>54640</v>
+        <v>499200</v>
       </c>
       <c r="CA2" t="n">
         <v>0</v>
@@ -1209,7 +1209,7 @@
         <v>37500</v>
       </c>
       <c r="AG3" t="n">
-        <v>1083660</v>
+        <v>1094172</v>
       </c>
       <c r="AH3" t="inlineStr"/>
       <c r="AI3" t="inlineStr"/>
@@ -1238,19 +1238,19 @@
         <v>1</v>
       </c>
       <c r="AR3" t="n">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="AS3" t="n">
-        <v>1084741</v>
+        <v>1095239</v>
       </c>
       <c r="AT3" t="n">
         <v>1</v>
       </c>
       <c r="AU3" t="n">
-        <v>68300</v>
+        <v>624000</v>
       </c>
       <c r="AV3" t="n">
-        <v>68300</v>
+        <v>624000</v>
       </c>
       <c r="AW3" t="n">
         <v>100</v>
@@ -1296,12 +1296,12 @@
       </c>
       <c r="BI3" t="inlineStr">
         <is>
-          <t>xqm242</t>
+          <t>xq03</t>
         </is>
       </c>
       <c r="BJ3" t="inlineStr">
         <is>
-          <t>Chụp Xquang cột sống cổ chếch hai bên</t>
+          <t>Chụp Xquang bể thận-niệu quản xuôi dòng [Số hóa]</t>
         </is>
       </c>
       <c r="BK3" t="inlineStr">
@@ -1340,13 +1340,13 @@
         <v>0</v>
       </c>
       <c r="BX3" t="n">
-        <v>13660</v>
+        <v>124800</v>
       </c>
       <c r="BY3" t="n">
         <v>0</v>
       </c>
       <c r="BZ3" t="n">
-        <v>54640</v>
+        <v>499200</v>
       </c>
       <c r="CA3" t="n">
         <v>0</v>

</xml_diff>